<commit_message>
Added binary logging to improve communication speed (to be tested).
</commit_message>
<xml_diff>
--- a/Hardware/BOM.xlsx
+++ b/Hardware/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unimelbcloud-my.sharepoint.com/personal/fong_j_unimelb_edu_au/Documents/FourierJointLab/ShoulderTrackingStudy/Tech/Hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{A725664C-4203-4E90-894B-EED76DF2B2B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EE4C17A6-143F-42FE-A089-E38241253899}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="13_ncr:1_{A725664C-4203-4E90-894B-EED76DF2B2B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E06799C2-4555-47A8-967A-9C5458FA16AF}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23076" windowHeight="9324" xr2:uid="{724A8CD7-7DD3-4B43-BCBE-89B5A2185EEF}"/>
+    <workbookView xWindow="11628" yWindow="2688" windowWidth="11424" windowHeight="9072" xr2:uid="{724A8CD7-7DD3-4B43-BCBE-89B5A2185EEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>Beetle BLE</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>SKU: POLOLU-2739</t>
+  </si>
+  <si>
+    <t>Stock</t>
   </si>
 </sst>
 </file>
@@ -251,7 +254,7 @@
     </xf>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -283,6 +286,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -600,26 +606,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{490E92A9-0967-44E7-AE34-EB1E5949F1F6}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="23.88671875" style="8" customWidth="1"/>
     <col min="2" max="2" width="15.5546875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="75.77734375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="45.77734375" style="8" customWidth="1"/>
     <col min="4" max="4" width="30.33203125" style="8" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" style="12" customWidth="1"/>
     <col min="6" max="6" width="9" style="8"/>
     <col min="7" max="7" width="10" style="8" customWidth="1"/>
-    <col min="8" max="8" width="23.88671875" style="8" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="8"/>
+    <col min="8" max="8" width="10" style="12" customWidth="1"/>
+    <col min="9" max="9" width="16" style="8" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -641,11 +648,14 @@
       <c r="G1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:10">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -659,17 +669,24 @@
         <v>25</v>
       </c>
       <c r="E2" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F2" s="5">
         <v>24.8</v>
       </c>
       <c r="G2" s="5">
         <f t="shared" ref="G2:G8" si="0">E2*F2</f>
-        <v>74.400000000000006</v>
+        <v>24.8</v>
+      </c>
+      <c r="H2" s="19">
+        <v>2</v>
+      </c>
+      <c r="J2" s="12">
+        <f>8-H2</f>
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:10">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -681,21 +698,28 @@
       </c>
       <c r="D3" s="13"/>
       <c r="E3" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F3" s="5">
         <v>9.9</v>
       </c>
       <c r="G3" s="5">
         <f>E3*F3</f>
-        <v>29.700000000000003</v>
-      </c>
-      <c r="H3" s="8">
+        <v>9.9</v>
+      </c>
+      <c r="H3" s="19">
+        <v>4</v>
+      </c>
+      <c r="I3" s="8">
         <f>SUM(G2:G3)</f>
-        <v>104.10000000000001</v>
+        <v>34.700000000000003</v>
+      </c>
+      <c r="J3" s="12">
+        <f>8-H3</f>
+        <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:10" ht="14.4" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -709,17 +733,24 @@
         <v>27</v>
       </c>
       <c r="E4" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F4" s="5">
         <v>2.15</v>
       </c>
       <c r="G4" s="5">
         <f t="shared" si="0"/>
-        <v>6.4499999999999993</v>
+        <v>2.15</v>
+      </c>
+      <c r="H4" s="19">
+        <v>3</v>
+      </c>
+      <c r="J4" s="12">
+        <f t="shared" ref="J3:J8" si="1">8-H4</f>
+        <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:10">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -733,17 +764,24 @@
         <v>31</v>
       </c>
       <c r="E5" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F5" s="5">
         <v>22.95</v>
       </c>
       <c r="G5" s="5">
         <f>E5*F5</f>
-        <v>68.849999999999994</v>
+        <v>22.95</v>
+      </c>
+      <c r="H5" s="19">
+        <v>2</v>
+      </c>
+      <c r="J5" s="12">
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:10">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -757,17 +795,24 @@
         <v>29</v>
       </c>
       <c r="E6" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F6" s="6">
         <v>3.22</v>
       </c>
       <c r="G6" s="5">
         <f t="shared" si="0"/>
-        <v>9.66</v>
+        <v>3.22</v>
+      </c>
+      <c r="H6" s="17">
+        <v>0</v>
+      </c>
+      <c r="J6" s="12">
+        <f t="shared" si="1"/>
+        <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:10">
       <c r="A7" s="16" t="s">
         <v>13</v>
       </c>
@@ -781,17 +826,24 @@
         <v>28</v>
       </c>
       <c r="E7" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F7" s="5">
         <v>12.46</v>
       </c>
       <c r="G7" s="5">
         <f t="shared" si="0"/>
-        <v>37.380000000000003</v>
+        <v>12.46</v>
+      </c>
+      <c r="H7" s="19">
+        <v>3</v>
+      </c>
+      <c r="J7" s="12">
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:10">
       <c r="A8" s="16" t="s">
         <v>15</v>
       </c>
@@ -805,17 +857,24 @@
         <v>26</v>
       </c>
       <c r="E8" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F8" s="5">
         <v>12.05</v>
       </c>
       <c r="G8" s="5">
         <f t="shared" si="0"/>
-        <v>36.150000000000006</v>
+        <v>12.05</v>
+      </c>
+      <c r="H8" s="19">
+        <v>4</v>
+      </c>
+      <c r="J8" s="12">
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:10">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -823,8 +882,9 @@
       <c r="E9" s="11"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
+      <c r="H9" s="19"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:10">
       <c r="A10" s="7" t="s">
         <v>17</v>
       </c>
@@ -838,11 +898,12 @@
       </c>
       <c r="G10" s="5">
         <f>SUM(G2:G9)</f>
-        <v>262.59000000000003</v>
-      </c>
-      <c r="H10" s="8">
-        <f>SUM(H2:H8)</f>
-        <v>104.10000000000001</v>
+        <v>87.529999999999987</v>
+      </c>
+      <c r="H10" s="19"/>
+      <c r="I10" s="8">
+        <f>SUM(I2:I8)</f>
+        <v>34.700000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>